<commit_message>
solucionar error en excel
</commit_message>
<xml_diff>
--- a/src/BBDD Prueba asincrónica.xlsx
+++ b/src/BBDD Prueba asincrónica.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basti\OneDrive\Escritorio\TareaInferenciaEstadistica\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324A5DD0-6066-4C44-B5CC-01EF0C2B0C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93F1B94-744C-4DFA-A8CC-48749BE4B98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="3675" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cuadro" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
   <dimension ref="A1:T268"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
-      <selection activeCell="C267" sqref="C267"/>
+      <selection activeCell="C269" sqref="C269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8661,8 +8661,8 @@
     </row>
     <row r="267" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A267">
-        <f>_xlfn.T.DIST(0.975,19,TRUE)</f>
-        <v>0.82909436237728174</v>
+        <f>_xlfn.T.INV(0.975,19)</f>
+        <v>2.0930240544083087</v>
       </c>
       <c r="B267" t="s">
         <v>10</v>
@@ -8681,11 +8681,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="857c3913-89a8-4469-a8ba-193410655798" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8827,20 +8828,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="857c3913-89a8-4469-a8ba-193410655798" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF334F9A-C47D-4588-97E5-1460B6982561}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A51CA5A7-7D8B-457A-8638-05A0D4A5DF70}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="857c3913-89a8-4469-a8ba-193410655798"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8864,9 +8862,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A51CA5A7-7D8B-457A-8638-05A0D4A5DF70}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF334F9A-C47D-4588-97E5-1460B6982561}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="857c3913-89a8-4469-a8ba-193410655798"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>